<commit_message>
saving so i can work on desktop
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Category</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Card</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>wads</t>
+  </si>
+  <si>
+    <t>453.0</t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -155,6 +164,23 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
added monthly total in report
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Category</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>2023-03-02</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>2023-03-22</t>
+  </si>
+  <si>
+    <t>123.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly total: </t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -237,6 +249,31 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5994.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -244,7 +281,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -284,6 +321,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="n">
+        <v>453.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
modified font styles and other things
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
-    <sheet name="april" r:id="rId4" sheetId="2"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>

<commit_message>
fixed bug where CSVReader didnt update when you logged out and logged into a new user
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
-    <sheet name="april" r:id="rId4" sheetId="2"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>

<commit_message>
adding progress to own branch so i can work on desktop
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -39,9 +39,6 @@
     <t>2023-03-20</t>
   </si>
   <si>
-    <t>432.0</t>
-  </si>
-  <si>
     <t>Savings</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>saw</t>
   </si>
   <si>
-    <t>4532.0</t>
-  </si>
-  <si>
     <t>Checkings</t>
   </si>
   <si>
@@ -69,49 +63,31 @@
     <t>2023-04-04</t>
   </si>
   <si>
-    <t>453.0</t>
-  </si>
-  <si>
     <t>dwads</t>
   </si>
   <si>
     <t>2023-03-01</t>
   </si>
   <si>
-    <t>43.0</t>
-  </si>
-  <si>
-    <t>dwas</t>
-  </si>
-  <si>
-    <t>2023-03-02</t>
+    <t>was</t>
+  </si>
+  <si>
+    <t>2023-04-12</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>msa, msaw, smw</t>
   </si>
   <si>
     <t>Transportation</t>
   </si>
   <si>
-    <t>2023-03-22</t>
-  </si>
-  <si>
-    <t>123.0</t>
-  </si>
-  <si>
-    <t>rgdf</t>
-  </si>
-  <si>
-    <t>2023-03-29</t>
-  </si>
-  <si>
-    <t>150.0</t>
-  </si>
-  <si>
-    <t>smws</t>
-  </si>
-  <si>
-    <t>200.0</t>
-  </si>
-  <si>
-    <t>ABC</t>
+    <t>smswa</t>
+  </si>
+  <si>
+    <t>smw, asmw, amws</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -159,7 +135,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -192,11 +168,11 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="n">
+        <v>432.0</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -204,33 +180,33 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3" t="n">
+        <v>432.0</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4532.0</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -238,92 +214,24 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="D5" t="n">
+        <v>43.0</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="n">
-        <v>6344.0</v>
+      <c r="B6" t="n">
+        <v>5439.0</v>
       </c>
     </row>
   </sheetData>
@@ -333,7 +241,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -361,24 +269,92 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D2" t="n">
+        <v>453.0</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="n">
-        <v>453.0</v>
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="n">
+        <v>342.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="n">
+        <v>405.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="n">
+        <v>405.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="n">
+        <v>501.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2106.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed barchart in overview window
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -6,14 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
-    <sheet name="april" r:id="rId4" sheetId="2"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>Category</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>smw, asmw, amws</t>
+  </si>
+  <si>
+    <t>rdfr</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>emsd</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -228,7 +237,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="n">
         <v>5439.0</v>
@@ -241,7 +250,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -351,10 +360,44 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="n">
-        <v>2106.0</v>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="n">
+        <v>656.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="n">
+        <v>450.0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3212.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error where expenses from previous months aren't added to the csv, because they dont appear in the table
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="April" r:id="rId3" sheetId="1"/>
+    <sheet name="March" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Category</t>
   </si>
@@ -29,31 +30,19 @@
     <t>Account</t>
   </si>
   <si>
-    <t>Food</t>
+    <t>Transportation</t>
   </si>
   <si>
-    <t>fgdr</t>
+    <t>ABC</t>
   </si>
   <si>
     <t>2023-04-14</t>
   </si>
   <si>
-    <t>Checkings</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>jnyg</t>
-  </si>
-  <si>
     <t>Savings</t>
   </si>
   <si>
-    <t>ABCD</t>
-  </si>
-  <si>
-    <t>ABC</t>
+    <t>2023-03-14</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -101,7 +90,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -135,7 +124,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>445.0</v>
+        <v>456.0</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -143,44 +132,65 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>456.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D2" t="n">
+        <v>456.0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1200.0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="n">
-        <v>500.0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2145.0</v>
+      <c r="B3" t="n">
+        <v>456.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug when reading csv file
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
-    <sheet name="april" r:id="rId4" sheetId="2"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>

<commit_message>
responsive piechart and total budget when removing or editing tables
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test.xlsx
+++ b/src/main/resources/userfiles/test/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Category</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>2023-04-21</t>
+  </si>
+  <si>
+    <t>fes</t>
+  </si>
+  <si>
+    <t>grd</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -183,7 +189,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" t="n">
         <v>999.0</v>
@@ -196,7 +202,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -366,7 +372,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="n">
-        <v>4000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -374,10 +380,44 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="n">
-        <v>9523.0</v>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="n">
+        <v>455.0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="n">
+        <v>546.0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="n">
+        <v>7524.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>